<commit_message>
the app should take data with multiple sheets now
</commit_message>
<xml_diff>
--- a/inst/extdata/infiltration_template.xlsx
+++ b/inst/extdata/infiltration_template.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccwrp.sharepoint.com/sites/Staff/Shared Documents/P Drive/Data/DuyNguyen/Projects/bmp-hydrology-calculator/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="11_69B14D2D7ECD495B2FBE795DDD970AF76451AD6D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B946084D-72D2-4276-810A-CCD4F5D816DD}"/>
+  <xr:revisionPtr revIDLastSave="51" documentId="11_69B14D2D7ECD495B2FBE795DDD970AF76451AD6D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836E81C9-80E7-484C-95B3-73083514DA68}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Storm Event 1" sheetId="1" r:id="rId2"/>
+    <sheet name="Storm Event 2" sheetId="9" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,15 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>datetime</t>
   </si>
   <si>
     <t>2021-12-14 05:14:00</t>
-  </si>
-  <si>
-    <t>DELETE THIS ROW TOO. It's only here for your preference what datatype that the app expects for each column</t>
   </si>
   <si>
     <t>Piezometer A</t>
@@ -55,6 +53,18 @@
   </si>
   <si>
     <t>Piezometer C</t>
+  </si>
+  <si>
+    <t>Delete this row too. It's only here for your preference what datatype that the app expects for each column. Please DO NOT delete/rename the datetime column</t>
+  </si>
+  <si>
+    <t>Sensor A</t>
+  </si>
+  <si>
+    <t>Sensor B</t>
+  </si>
+  <si>
+    <t>Sensor C</t>
   </si>
 </sst>
 </file>
@@ -425,7 +435,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65AA0D0C-9576-42E0-B206-BB50AFF0F4EA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -440,11 +452,11 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +464,7 @@
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="146.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -460,13 +472,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -483,12 +495,64 @@
         <v>23.75</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24AA02F9-74E8-4B1F-B780-555BEF4CA6AF}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="146.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="3" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
+        <v>50.17</v>
+      </c>
+      <c r="C2" s="4">
+        <v>24.88</v>
+      </c>
+      <c r="D2" s="4">
+        <v>23.75</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -767,15 +831,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2">
@@ -787,6 +842,15 @@
     <OldForms xmlns="02ea596c-bf3f-4512-ad68-024a720c79b2" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -810,14 +874,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F491C895-60B5-42FC-B899-C02C4CA1FC39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1D4CCFB-8D37-4996-95ED-94B4EFCE2A00}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -835,4 +891,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F491C895-60B5-42FC-B899-C02C4CA1FC39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>